<commit_message>
Import Student Numbers from spraedsheet
</commit_message>
<xml_diff>
--- a/test/fixtures/people-import--single-primary.xlsx
+++ b/test/fixtures/people-import--single-primary.xlsx
@@ -8,11 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Export_for_Ballistiq" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Export for Ballistiq" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="false" name="Export_for_Ballistiq" vbProcedure="false">Export_for_Ballistiq!$A$1:$BE$2</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -23,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
   <si>
     <t xml:space="preserve">Last</t>
   </si>
@@ -196,13 +193,16 @@
     <t xml:space="preserve">Conference Status</t>
   </si>
   <si>
+    <t xml:space="preserve">Student Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abbott</t>
   </si>
   <si>
     <t xml:space="preserve">Duane</t>
   </si>
   <si>
-    <t xml:space="preserve">Abbott-0638533</t>
+    <t xml:space="preserve">Abbott-65ad</t>
   </si>
   <si>
     <t xml:space="preserve">Primary</t>
@@ -214,6 +214,12 @@
     <t xml:space="preserve">0638533</t>
   </si>
   <si>
+    <t xml:space="preserve">Men's 2XL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No.</t>
+  </si>
+  <si>
     <t xml:space="preserve">114 Mountain Valley Dr</t>
   </si>
   <si>
@@ -223,16 +229,28 @@
     <t xml:space="preserve">AR</t>
   </si>
   <si>
-    <t xml:space="preserve">72113-6993</t>
+    <t xml:space="preserve">72113</t>
   </si>
   <si>
     <t xml:space="preserve">USA</t>
   </si>
   <si>
-    <t xml:space="preserve">515/473-8402</t>
+    <t xml:space="preserve">5154738402</t>
   </si>
   <si>
     <t xml:space="preserve">dabbott@familylife.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cru17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Off Campus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">FL33230</t>
@@ -247,7 +265,7 @@
     <t xml:space="preserve">STFFD.LH.STAFF</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-registered Import</t>
+    <t xml:space="preserve">Registered</t>
   </si>
 </sst>
 </file>
@@ -256,13 +274,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="DD/MMM/YY"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -285,28 +303,28 @@
       <b val="true"/>
       <sz val="24"/>
       <color rgb="FF000000"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -314,28 +332,28 @@
       <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -343,7 +361,7 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -351,19 +369,34 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,11 +442,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFD0D7E5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFD0D7E5"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -433,6 +472,28 @@
       </top>
       <bottom style="thin">
         <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFD0D7E5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD0D7E5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD0D7E5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0D7E5"/>
       </bottom>
       <diagonal/>
     </border>
@@ -510,17 +571,29 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -569,11 +642,11 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFD0D7E5"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -616,7 +689,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BE65536"/>
+  <dimension ref="A1:BF65536"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -624,250 +697,1303 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="1" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="59" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BC1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BD1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BE1" s="2" t="s">
         <v>56</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>57</v>
+      <c r="D2" s="3" t="s">
+        <v>61</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>61</v>
+      <c r="F2" s="3" t="s">
+        <v>59</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="H2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="4" t="n">
         <v>24602</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>63</v>
+      <c r="J2" s="5" t="n">
+        <v>50</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="O2" s="3"/>
+      <c r="P2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="Q2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="R2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="S2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="T2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AY2" s="2" t="n">
+      <c r="U2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="W2" s="3"/>
+      <c r="X2" s="4" t="n">
+        <v>42931</v>
+      </c>
+      <c r="Y2" s="4" t="n">
+        <v>42940</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN2" s="3"/>
+      <c r="AP2" s="3"/>
+      <c r="AQ2" s="3"/>
+      <c r="AR2" s="3"/>
+      <c r="AS2" s="3"/>
+      <c r="AT2" s="3"/>
+      <c r="AU2" s="4" t="n">
+        <v>42933</v>
+      </c>
+      <c r="AV2" s="4" t="n">
+        <v>42939</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY2" s="4" t="n">
         <v>40940</v>
       </c>
-      <c r="AZ2" s="1" t="s">
-        <v>72</v>
+      <c r="AZ2" s="3" t="s">
+        <v>79</v>
       </c>
-      <c r="BD2" s="1" t="s">
-        <v>73</v>
+      <c r="BA2" s="3"/>
+      <c r="BB2" s="3"/>
+      <c r="BC2" s="3"/>
+      <c r="BD2" s="3" t="s">
+        <v>80</v>
       </c>
-      <c r="BE2" s="1" t="s">
-        <v>74</v>
+      <c r="BE2" s="3" t="s">
+        <v>81</v>
       </c>
+      <c r="BF2" s="3"/>
     </row>
+    <row r="1040383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040587" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040588" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040589" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040590" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040591" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040592" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040593" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040596" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040597" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040598" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040599" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040601" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040602" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040604" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040605" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040606" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040607" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040609" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040618" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040619" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040620" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040621" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040622" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040623" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040624" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040625" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040626" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040627" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040628" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040630" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040631" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040632" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040633" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040634" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040635" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040636" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040637" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040638" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040640" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040642" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040643" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040644" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040645" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040646" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040647" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040648" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040649" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040650" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040651" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040652" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040653" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040654" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040655" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040656" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040657" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040658" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040659" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040660" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040661" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040662" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040663" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040664" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040665" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040666" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040667" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040668" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040669" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040670" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040671" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040672" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040673" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040674" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040675" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040676" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040677" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040678" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040679" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040680" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040681" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040682" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040683" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040684" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040685" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040686" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040687" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040688" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040689" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040690" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040691" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040692" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040693" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040694" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040695" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040696" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040697" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040698" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040699" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040700" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040701" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040702" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040703" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040704" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040705" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040706" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040707" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040708" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040709" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040710" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040711" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040712" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040713" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040714" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040715" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040716" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040717" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040718" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040719" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040720" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040721" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040722" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040723" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040724" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040725" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040726" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040727" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040728" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040729" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040730" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040731" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040732" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040733" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040734" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040735" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040736" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040738" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040745" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040746" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040747" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040748" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040749" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040750" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040751" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040752" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040753" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040755" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040756" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040757" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040759" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040760" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040761" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040762" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040763" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040764" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040765" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040766" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040767" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040768" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040769" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040770" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040771" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040772" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040773" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040774" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040775" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040776" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040777" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040778" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040779" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040780" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040781" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040782" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040783" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040784" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040785" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040786" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040787" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040788" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040789" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040790" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040791" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040792" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040793" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040794" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040795" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040796" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040797" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040798" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040799" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040800" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040801" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040802" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040803" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040804" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040805" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040806" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040807" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040808" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040809" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040810" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040811" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040812" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040813" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040814" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040815" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040816" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040817" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040818" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040819" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040820" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040821" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040822" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040823" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040824" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040825" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040826" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040827" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040828" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040829" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040830" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040831" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040832" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040833" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040834" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040835" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040836" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040837" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040838" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040839" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040840" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040841" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040842" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040843" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040844" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040845" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040846" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040847" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040848" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040849" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040850" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040851" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040852" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040853" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040854" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040855" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040856" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040857" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040858" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040859" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040860" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040861" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040862" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040863" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040864" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040865" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040866" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040867" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040868" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040869" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040870" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040871" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040872" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040873" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040874" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040875" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040876" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040877" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040878" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040879" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040880" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040881" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040882" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040883" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040884" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040885" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040886" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040887" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040888" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040890" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040891" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040892" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040893" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040894" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040895" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040896" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040897" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040898" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040899" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040900" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040901" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040902" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040903" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040904" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040905" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040906" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040907" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040908" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040909" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040910" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040911" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040912" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040913" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040914" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040915" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040916" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040917" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040918" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040921" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040922" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040923" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040924" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040925" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040926" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040927" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040928" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040929" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040930" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040931" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040932" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040933" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040934" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040935" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040936" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040937" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040938" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040939" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040940" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040941" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040942" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040943" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040944" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040945" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040946" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040947" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040948" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040949" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040950" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040951" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040952" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040953" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040954" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040955" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040956" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040957" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040958" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040959" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040960" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040961" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040962" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040963" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040964" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040965" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040966" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040967" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040968" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040969" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040970" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040971" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040972" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040973" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040974" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040975" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040976" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040977" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040978" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040979" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040980" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040981" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040982" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040983" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040984" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040985" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040986" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040987" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040988" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040989" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040990" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040992" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040993" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040994" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041000" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041001" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041002" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041003" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041004" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041005" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041006" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041007" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041008" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041009" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041010" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041011" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041012" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041013" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041014" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041015" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041016" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041017" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041018" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041019" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041020" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041021" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041022" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041023" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041024" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041025" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041026" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041027" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041028" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041029" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041030" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041031" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041032" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041033" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041034" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041035" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041036" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041037" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041038" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041039" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041040" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041041" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041042" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041043" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041044" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041045" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041046" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041047" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041048" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041049" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041050" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041051" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041052" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041053" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041054" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041055" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041056" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041057" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041058" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041059" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041060" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041061" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041062" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041063" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041064" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041065" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041066" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041067" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041068" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041069" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041070" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041071" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041072" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041073" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041074" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041075" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041076" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041077" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041078" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041079" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041080" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041081" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041082" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041083" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041084" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041085" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041086" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041087" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041088" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041089" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041090" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041091" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041092" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041093" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041094" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041095" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041096" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041097" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041098" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041099" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1041377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1041378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1041379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>